<commit_message>
Milira Event Story Expand The Tale of Milira - 3477405110
</commit_message>
<xml_diff>
--- a/Data/Milira Event Story Expand The Tale of Milira - 3477405110/Milira Event Story Expand The Tale of Milira - 3477405110.xlsx
+++ b/Data/Milira Event Story Expand The Tale of Milira - 3477405110/Milira Event Story Expand The Tale of Milira - 3477405110.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\optol\OneDrive\바탕 화면\rimpy\translate\완성\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\optol\OneDrive\바탕 화면\rimpy\translate\임시\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84687489-50CA-4EF6-9451-DFC76FF5880E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9D18EA2-4BE7-4DC1-9E6C-2402C985CD1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15210" yWindow="9210" windowWidth="32310" windowHeight="18690" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5085" yWindow="1515" windowWidth="32310" windowHeight="19455" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -4572,9 +4572,6 @@
     <t>보급품 투하 지점 발견 - 생산 자재</t>
   </si>
   <si>
-    <t>밀리라 거점의 위치 노출을 피하기 위해, 그들의 보급품은 바로 머리 위에 공중 투하되지 않는다고 합니다. 우리가 좌표를 따라가자, 밀리라가 사용하는 각종 자재들이 흩어진 것을 발견했습니다.\n\n-셀레스티움 합금 직물\n-태양 단조강\n-밀리라 핵심 부품\n\n주의해야 합니다. 보급품이 발산한 신호가 다른 약탈자들을 끌어들였을 수 있습니다.</t>
-  </si>
-  <si>
     <t>자재들을 포장하며 전투 태세를 갖춘다</t>
   </si>
   <si>
@@ -5028,6 +5025,9 @@
   <si>
     <t>TheTaleOfMilira_Event_TheMiliraSupply.root.nodes.WorldObjectTimeout.node.nodes.Letter.text</t>
     <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>밀리라 거점의 위치 노출을 피하기 위해, 그들의 보급품은 바로 머리 위에 공중 투하되지 않는다고 합니다. 우리가 좌표를 따라가자, 밀리라가 사용하는 각종 자재들이 흩어진 것을 발견했습니다.\n\n-셀레스티움 합금 직물\n-태양단강\n-밀리라 핵심 부품\n\n주의해야 합니다. 보급품이 발산한 신호가 다른 약탈자들을 끌어들였을 수 있습니다.</t>
   </si>
 </sst>
 </file>
@@ -5383,7 +5383,7 @@
   <dimension ref="A1:F462"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="S33" sqref="S33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5391,7 +5391,7 @@
     <col min="1" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5411,7 +5411,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -5429,7 +5429,7 @@
         <v>1329</v>
       </c>
     </row>
-    <row r="3" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
@@ -5447,7 +5447,7 @@
         <v>1330</v>
       </c>
     </row>
-    <row r="4" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>13</v>
       </c>
@@ -5465,7 +5465,7 @@
         <v>1269</v>
       </c>
     </row>
-    <row r="5" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>16</v>
       </c>
@@ -5483,7 +5483,7 @@
         <v>1329</v>
       </c>
     </row>
-    <row r="6" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>18</v>
       </c>
@@ -5501,7 +5501,7 @@
         <v>1330</v>
       </c>
     </row>
-    <row r="7" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>20</v>
       </c>
@@ -5519,7 +5519,7 @@
         <v>1270</v>
       </c>
     </row>
-    <row r="8" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>23</v>
       </c>
@@ -5537,7 +5537,7 @@
         <v>1331</v>
       </c>
     </row>
-    <row r="9" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>26</v>
       </c>
@@ -5555,7 +5555,7 @@
         <v>1332</v>
       </c>
     </row>
-    <row r="10" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>29</v>
       </c>
@@ -5573,7 +5573,7 @@
         <v>1271</v>
       </c>
     </row>
-    <row r="11" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>32</v>
       </c>
@@ -5591,7 +5591,7 @@
         <v>1333</v>
       </c>
     </row>
-    <row r="12" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>35</v>
       </c>
@@ -5609,7 +5609,7 @@
         <v>1334</v>
       </c>
     </row>
-    <row r="13" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>38</v>
       </c>
@@ -5627,7 +5627,7 @@
         <v>1272</v>
       </c>
     </row>
-    <row r="14" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>41</v>
       </c>
@@ -5645,7 +5645,7 @@
         <v>1335</v>
       </c>
     </row>
-    <row r="15" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>44</v>
       </c>
@@ -5663,7 +5663,7 @@
         <v>1336</v>
       </c>
     </row>
-    <row r="16" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>47</v>
       </c>
@@ -5681,7 +5681,7 @@
         <v>1273</v>
       </c>
     </row>
-    <row r="17" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>50</v>
       </c>
@@ -5699,7 +5699,7 @@
         <v>1335</v>
       </c>
     </row>
-    <row r="18" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>52</v>
       </c>
@@ -5717,7 +5717,7 @@
         <v>1336</v>
       </c>
     </row>
-    <row r="19" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>54</v>
       </c>
@@ -5735,7 +5735,7 @@
         <v>1274</v>
       </c>
     </row>
-    <row r="20" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>57</v>
       </c>
@@ -5753,7 +5753,7 @@
         <v>1329</v>
       </c>
     </row>
-    <row r="21" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>59</v>
       </c>
@@ -5771,7 +5771,7 @@
         <v>1330</v>
       </c>
     </row>
-    <row r="22" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>61</v>
       </c>
@@ -5789,7 +5789,7 @@
         <v>1275</v>
       </c>
     </row>
-    <row r="23" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>63</v>
       </c>
@@ -5807,7 +5807,7 @@
         <v>1335</v>
       </c>
     </row>
-    <row r="24" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>65</v>
       </c>
@@ -5825,7 +5825,7 @@
         <v>1336</v>
       </c>
     </row>
-    <row r="25" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>67</v>
       </c>
@@ -5843,7 +5843,7 @@
         <v>1276</v>
       </c>
     </row>
-    <row r="26" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>70</v>
       </c>
@@ -5861,7 +5861,7 @@
         <v>1337</v>
       </c>
     </row>
-    <row r="27" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>73</v>
       </c>
@@ -5879,7 +5879,7 @@
         <v>1338</v>
       </c>
     </row>
-    <row r="28" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>76</v>
       </c>
@@ -5894,10 +5894,10 @@
         <v>69</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>1529</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+        <v>1528</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>78</v>
       </c>
@@ -5915,7 +5915,7 @@
         <v>1339</v>
       </c>
     </row>
-    <row r="30" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>81</v>
       </c>
@@ -5933,7 +5933,7 @@
         <v>1340</v>
       </c>
     </row>
-    <row r="31" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>84</v>
       </c>
@@ -5948,10 +5948,10 @@
         <v>1277</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>1528</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+        <v>1527</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>86</v>
       </c>
@@ -5969,7 +5969,7 @@
         <v>1341</v>
       </c>
     </row>
-    <row r="33" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>89</v>
       </c>
@@ -5987,7 +5987,7 @@
         <v>1342</v>
       </c>
     </row>
-    <row r="34" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>92</v>
       </c>
@@ -6005,7 +6005,7 @@
         <v>1278</v>
       </c>
     </row>
-    <row r="35" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>95</v>
       </c>
@@ -6023,7 +6023,7 @@
         <v>1343</v>
       </c>
     </row>
-    <row r="36" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>98</v>
       </c>
@@ -6041,7 +6041,7 @@
         <v>1344</v>
       </c>
     </row>
-    <row r="37" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>101</v>
       </c>
@@ -6059,7 +6059,7 @@
         <v>1279</v>
       </c>
     </row>
-    <row r="38" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>104</v>
       </c>
@@ -6077,7 +6077,7 @@
         <v>1345</v>
       </c>
     </row>
-    <row r="39" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>107</v>
       </c>
@@ -6095,7 +6095,7 @@
         <v>1346</v>
       </c>
     </row>
-    <row r="40" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>110</v>
       </c>
@@ -6113,7 +6113,7 @@
         <v>1347</v>
       </c>
     </row>
-    <row r="41" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>113</v>
       </c>
@@ -6131,7 +6131,7 @@
         <v>1348</v>
       </c>
     </row>
-    <row r="42" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
         <v>116</v>
       </c>
@@ -6149,7 +6149,7 @@
         <v>1349</v>
       </c>
     </row>
-    <row r="43" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
         <v>119</v>
       </c>
@@ -6167,7 +6167,7 @@
         <v>1280</v>
       </c>
     </row>
-    <row r="44" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>122</v>
       </c>
@@ -6185,7 +6185,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="45" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
         <v>125</v>
       </c>
@@ -6203,7 +6203,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="46" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
         <v>128</v>
       </c>
@@ -6221,7 +6221,7 @@
         <v>1281</v>
       </c>
     </row>
-    <row r="47" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
         <v>131</v>
       </c>
@@ -6239,7 +6239,7 @@
         <v>1352</v>
       </c>
     </row>
-    <row r="48" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
         <v>134</v>
       </c>
@@ -6257,7 +6257,7 @@
         <v>1353</v>
       </c>
     </row>
-    <row r="49" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
         <v>137</v>
       </c>
@@ -6275,7 +6275,7 @@
         <v>1282</v>
       </c>
     </row>
-    <row r="50" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
         <v>140</v>
       </c>
@@ -6293,7 +6293,7 @@
         <v>1354</v>
       </c>
     </row>
-    <row r="51" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
         <v>143</v>
       </c>
@@ -6311,7 +6311,7 @@
         <v>1355</v>
       </c>
     </row>
-    <row r="52" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
         <v>146</v>
       </c>
@@ -6329,7 +6329,7 @@
         <v>1283</v>
       </c>
     </row>
-    <row r="53" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
         <v>149</v>
       </c>
@@ -6347,7 +6347,7 @@
         <v>1356</v>
       </c>
     </row>
-    <row r="54" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
         <v>152</v>
       </c>
@@ -6365,7 +6365,7 @@
         <v>1357</v>
       </c>
     </row>
-    <row r="55" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
         <v>155</v>
       </c>
@@ -6383,7 +6383,7 @@
         <v>1284</v>
       </c>
     </row>
-    <row r="56" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
         <v>158</v>
       </c>
@@ -6401,7 +6401,7 @@
         <v>1358</v>
       </c>
     </row>
-    <row r="57" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
         <v>161</v>
       </c>
@@ -6419,7 +6419,7 @@
         <v>1359</v>
       </c>
     </row>
-    <row r="58" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
         <v>164</v>
       </c>
@@ -6437,7 +6437,7 @@
         <v>1360</v>
       </c>
     </row>
-    <row r="59" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
         <v>166</v>
       </c>
@@ -6455,7 +6455,7 @@
         <v>1361</v>
       </c>
     </row>
-    <row r="60" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
         <v>169</v>
       </c>
@@ -6473,7 +6473,7 @@
         <v>1362</v>
       </c>
     </row>
-    <row r="61" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
         <v>172</v>
       </c>
@@ -6491,7 +6491,7 @@
         <v>1285</v>
       </c>
     </row>
-    <row r="62" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
         <v>175</v>
       </c>
@@ -6509,7 +6509,7 @@
         <v>1344</v>
       </c>
     </row>
-    <row r="63" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
         <v>178</v>
       </c>
@@ -6527,7 +6527,7 @@
         <v>1363</v>
       </c>
     </row>
-    <row r="64" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
         <v>181</v>
       </c>
@@ -6545,7 +6545,7 @@
         <v>1363</v>
       </c>
     </row>
-    <row r="65" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
         <v>183</v>
       </c>
@@ -6563,7 +6563,7 @@
         <v>1341</v>
       </c>
     </row>
-    <row r="66" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
         <v>186</v>
       </c>
@@ -6581,7 +6581,7 @@
         <v>1335</v>
       </c>
     </row>
-    <row r="67" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
         <v>189</v>
       </c>
@@ -6599,7 +6599,7 @@
         <v>1364</v>
       </c>
     </row>
-    <row r="68" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
         <v>192</v>
       </c>
@@ -6617,7 +6617,7 @@
         <v>1365</v>
       </c>
     </row>
-    <row r="69" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
         <v>195</v>
       </c>
@@ -6635,7 +6635,7 @@
         <v>1366</v>
       </c>
     </row>
-    <row r="70" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
         <v>198</v>
       </c>
@@ -6653,7 +6653,7 @@
         <v>1367</v>
       </c>
     </row>
-    <row r="71" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
         <v>201</v>
       </c>
@@ -6671,7 +6671,7 @@
         <v>1368</v>
       </c>
     </row>
-    <row r="72" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="s">
         <v>204</v>
       </c>
@@ -6689,7 +6689,7 @@
         <v>1369</v>
       </c>
     </row>
-    <row r="73" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
         <v>208</v>
       </c>
@@ -6707,7 +6707,7 @@
         <v>1286</v>
       </c>
     </row>
-    <row r="74" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
         <v>211</v>
       </c>
@@ -6723,7 +6723,7 @@
       </c>
       <c r="F74" s="1"/>
     </row>
-    <row r="75" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A75" s="1" t="s">
         <v>214</v>
       </c>
@@ -6739,7 +6739,7 @@
       </c>
       <c r="F75" s="1"/>
     </row>
-    <row r="76" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="s">
         <v>217</v>
       </c>
@@ -6747,7 +6747,7 @@
         <v>205</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>1619</v>
+        <v>1618</v>
       </c>
       <c r="D76" s="1"/>
       <c r="E76" s="1" t="s">
@@ -6757,7 +6757,7 @@
         <v>1370</v>
       </c>
     </row>
-    <row r="77" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A77" s="1" t="s">
         <v>219</v>
       </c>
@@ -6765,7 +6765,7 @@
         <v>205</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>1620</v>
+        <v>1619</v>
       </c>
       <c r="D77" s="1"/>
       <c r="E77" s="1" t="s">
@@ -6775,7 +6775,7 @@
         <v>1371</v>
       </c>
     </row>
-    <row r="78" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A78" s="1" t="s">
         <v>221</v>
       </c>
@@ -6793,7 +6793,7 @@
         <v>1372</v>
       </c>
     </row>
-    <row r="79" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A79" s="1" t="s">
         <v>224</v>
       </c>
@@ -6811,7 +6811,7 @@
         <v>1287</v>
       </c>
     </row>
-    <row r="80" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A80" s="1" t="s">
         <v>227</v>
       </c>
@@ -6827,7 +6827,7 @@
       </c>
       <c r="F80" s="1"/>
     </row>
-    <row r="81" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A81" s="1" t="s">
         <v>229</v>
       </c>
@@ -6843,7 +6843,7 @@
       </c>
       <c r="F81" s="1"/>
     </row>
-    <row r="82" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A82" s="1" t="s">
         <v>231</v>
       </c>
@@ -6851,7 +6851,7 @@
         <v>205</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>1621</v>
+        <v>1620</v>
       </c>
       <c r="D82" s="1"/>
       <c r="E82" s="1" t="s">
@@ -6861,7 +6861,7 @@
         <v>1370</v>
       </c>
     </row>
-    <row r="83" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A83" s="1" t="s">
         <v>232</v>
       </c>
@@ -6869,7 +6869,7 @@
         <v>205</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>1622</v>
+        <v>1621</v>
       </c>
       <c r="D83" s="1"/>
       <c r="E83" s="1" t="s">
@@ -6879,7 +6879,7 @@
         <v>1373</v>
       </c>
     </row>
-    <row r="84" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A84" s="1" t="s">
         <v>234</v>
       </c>
@@ -6897,7 +6897,7 @@
         <v>1374</v>
       </c>
     </row>
-    <row r="85" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A85" s="1" t="s">
         <v>237</v>
       </c>
@@ -6915,7 +6915,7 @@
         <v>1375</v>
       </c>
     </row>
-    <row r="86" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A86" s="1" t="s">
         <v>240</v>
       </c>
@@ -6931,7 +6931,7 @@
       </c>
       <c r="F86" s="1"/>
     </row>
-    <row r="87" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A87" s="1" t="s">
         <v>242</v>
       </c>
@@ -6947,7 +6947,7 @@
       </c>
       <c r="F87" s="1"/>
     </row>
-    <row r="88" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A88" s="1" t="s">
         <v>244</v>
       </c>
@@ -6955,7 +6955,7 @@
         <v>205</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>1623</v>
+        <v>1622</v>
       </c>
       <c r="D88" s="1"/>
       <c r="E88" s="1" t="s">
@@ -6965,7 +6965,7 @@
         <v>1370</v>
       </c>
     </row>
-    <row r="89" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A89" s="1" t="s">
         <v>245</v>
       </c>
@@ -6973,7 +6973,7 @@
         <v>205</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>1624</v>
+        <v>1623</v>
       </c>
       <c r="D89" s="1"/>
       <c r="E89" s="1" t="s">
@@ -6983,7 +6983,7 @@
         <v>1376</v>
       </c>
     </row>
-    <row r="90" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A90" s="1" t="s">
         <v>247</v>
       </c>
@@ -7001,7 +7001,7 @@
         <v>1377</v>
       </c>
     </row>
-    <row r="91" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A91" s="1" t="s">
         <v>250</v>
       </c>
@@ -7019,7 +7019,7 @@
         <v>1378</v>
       </c>
     </row>
-    <row r="92" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A92" s="1" t="s">
         <v>253</v>
       </c>
@@ -7035,7 +7035,7 @@
       </c>
       <c r="F92" s="1"/>
     </row>
-    <row r="93" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A93" s="1" t="s">
         <v>255</v>
       </c>
@@ -7051,7 +7051,7 @@
       </c>
       <c r="F93" s="1"/>
     </row>
-    <row r="94" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A94" s="1" t="s">
         <v>257</v>
       </c>
@@ -7059,7 +7059,7 @@
         <v>205</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>1625</v>
+        <v>1624</v>
       </c>
       <c r="D94" s="1"/>
       <c r="E94" s="1" t="s">
@@ -7069,7 +7069,7 @@
         <v>1370</v>
       </c>
     </row>
-    <row r="95" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A95" s="1" t="s">
         <v>258</v>
       </c>
@@ -7077,7 +7077,7 @@
         <v>205</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>1626</v>
+        <v>1625</v>
       </c>
       <c r="D95" s="1"/>
       <c r="E95" s="1" t="s">
@@ -7087,7 +7087,7 @@
         <v>1379</v>
       </c>
     </row>
-    <row r="96" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A96" s="1" t="s">
         <v>260</v>
       </c>
@@ -7105,7 +7105,7 @@
         <v>1380</v>
       </c>
     </row>
-    <row r="97" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A97" s="1" t="s">
         <v>263</v>
       </c>
@@ -7120,10 +7120,10 @@
         <v>265</v>
       </c>
       <c r="F97" s="1" t="s">
-        <v>1617</v>
-      </c>
-    </row>
-    <row r="98" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+        <v>1616</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A98" s="1" t="s">
         <v>266</v>
       </c>
@@ -7139,7 +7139,7 @@
       </c>
       <c r="F98" s="1"/>
     </row>
-    <row r="99" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A99" s="1" t="s">
         <v>268</v>
       </c>
@@ -7155,7 +7155,7 @@
       </c>
       <c r="F99" s="1"/>
     </row>
-    <row r="100" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A100" s="1" t="s">
         <v>270</v>
       </c>
@@ -7163,7 +7163,7 @@
         <v>205</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>1627</v>
+        <v>1626</v>
       </c>
       <c r="D100" s="1"/>
       <c r="E100" s="1" t="s">
@@ -7173,7 +7173,7 @@
         <v>1370</v>
       </c>
     </row>
-    <row r="101" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A101" s="1" t="s">
         <v>271</v>
       </c>
@@ -7181,7 +7181,7 @@
         <v>205</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>1628</v>
+        <v>1627</v>
       </c>
       <c r="D101" s="1"/>
       <c r="E101" s="1" t="s">
@@ -7191,7 +7191,7 @@
         <v>1381</v>
       </c>
     </row>
-    <row r="102" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A102" s="1" t="s">
         <v>273</v>
       </c>
@@ -7209,7 +7209,7 @@
         <v>1380</v>
       </c>
     </row>
-    <row r="103" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A103" s="1" t="s">
         <v>275</v>
       </c>
@@ -7224,10 +7224,10 @@
         <v>277</v>
       </c>
       <c r="F103" s="1" t="s">
-        <v>1618</v>
-      </c>
-    </row>
-    <row r="104" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+        <v>1617</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A104" s="1" t="s">
         <v>278</v>
       </c>
@@ -7243,7 +7243,7 @@
       </c>
       <c r="F104" s="1"/>
     </row>
-    <row r="105" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A105" s="1" t="s">
         <v>280</v>
       </c>
@@ -7259,7 +7259,7 @@
       </c>
       <c r="F105" s="1"/>
     </row>
-    <row r="106" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A106" s="1" t="s">
         <v>282</v>
       </c>
@@ -7267,7 +7267,7 @@
         <v>205</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>1629</v>
+        <v>1628</v>
       </c>
       <c r="D106" s="1"/>
       <c r="E106" s="1" t="s">
@@ -7277,7 +7277,7 @@
         <v>1370</v>
       </c>
     </row>
-    <row r="107" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A107" s="1" t="s">
         <v>283</v>
       </c>
@@ -7285,7 +7285,7 @@
         <v>205</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>1632</v>
+        <v>1631</v>
       </c>
       <c r="D107" s="1"/>
       <c r="E107" s="1" t="s">
@@ -7295,7 +7295,7 @@
         <v>1381</v>
       </c>
     </row>
-    <row r="108" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A108" s="1" t="s">
         <v>285</v>
       </c>
@@ -7313,7 +7313,7 @@
         <v>1382</v>
       </c>
     </row>
-    <row r="109" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A109" s="1" t="s">
         <v>288</v>
       </c>
@@ -7331,7 +7331,7 @@
         <v>1375</v>
       </c>
     </row>
-    <row r="110" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A110" s="1" t="s">
         <v>291</v>
       </c>
@@ -7347,7 +7347,7 @@
       </c>
       <c r="F110" s="1"/>
     </row>
-    <row r="111" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A111" s="1" t="s">
         <v>293</v>
       </c>
@@ -7363,7 +7363,7 @@
       </c>
       <c r="F111" s="1"/>
     </row>
-    <row r="112" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A112" s="1" t="s">
         <v>295</v>
       </c>
@@ -7371,7 +7371,7 @@
         <v>205</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>1630</v>
+        <v>1629</v>
       </c>
       <c r="D112" s="1"/>
       <c r="E112" s="1" t="s">
@@ -7381,7 +7381,7 @@
         <v>1370</v>
       </c>
     </row>
-    <row r="113" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A113" s="1" t="s">
         <v>296</v>
       </c>
@@ -7389,7 +7389,7 @@
         <v>205</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>1631</v>
+        <v>1630</v>
       </c>
       <c r="D113" s="1"/>
       <c r="E113" s="1" t="s">
@@ -7399,7 +7399,7 @@
         <v>1376</v>
       </c>
     </row>
-    <row r="114" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A114" s="1" t="s">
         <v>297</v>
       </c>
@@ -7417,7 +7417,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="115" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A115" s="1" t="s">
         <v>301</v>
       </c>
@@ -7435,7 +7435,7 @@
         <v>1383</v>
       </c>
     </row>
-    <row r="116" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A116" s="1" t="s">
         <v>305</v>
       </c>
@@ -7453,7 +7453,7 @@
         <v>1384</v>
       </c>
     </row>
-    <row r="117" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A117" s="1" t="s">
         <v>308</v>
       </c>
@@ -7471,7 +7471,7 @@
         <v>1385</v>
       </c>
     </row>
-    <row r="118" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A118" s="1" t="s">
         <v>311</v>
       </c>
@@ -7489,7 +7489,7 @@
         <v>1386</v>
       </c>
     </row>
-    <row r="119" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A119" s="1" t="s">
         <v>315</v>
       </c>
@@ -7507,7 +7507,7 @@
         <v>1387</v>
       </c>
     </row>
-    <row r="120" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A120" s="1" t="s">
         <v>318</v>
       </c>
@@ -7525,7 +7525,7 @@
         <v>1388</v>
       </c>
     </row>
-    <row r="121" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A121" s="1" t="s">
         <v>321</v>
       </c>
@@ -7543,7 +7543,7 @@
         <v>1389</v>
       </c>
     </row>
-    <row r="122" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A122" s="1" t="s">
         <v>324</v>
       </c>
@@ -7561,7 +7561,7 @@
         <v>1390</v>
       </c>
     </row>
-    <row r="123" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A123" s="1" t="s">
         <v>327</v>
       </c>
@@ -7579,7 +7579,7 @@
         <v>1391</v>
       </c>
     </row>
-    <row r="124" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A124" s="1" t="s">
         <v>330</v>
       </c>
@@ -7597,7 +7597,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="125" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A125" s="1" t="s">
         <v>333</v>
       </c>
@@ -7615,7 +7615,7 @@
         <v>1393</v>
       </c>
     </row>
-    <row r="126" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A126" s="1" t="s">
         <v>335</v>
       </c>
@@ -7633,7 +7633,7 @@
         <v>1394</v>
       </c>
     </row>
-    <row r="127" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A127" s="1" t="s">
         <v>338</v>
       </c>
@@ -7651,7 +7651,7 @@
         <v>1395</v>
       </c>
     </row>
-    <row r="128" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A128" s="1" t="s">
         <v>341</v>
       </c>
@@ -7669,7 +7669,7 @@
         <v>1396</v>
       </c>
     </row>
-    <row r="129" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A129" s="1" t="s">
         <v>344</v>
       </c>
@@ -7687,7 +7687,7 @@
         <v>1397</v>
       </c>
     </row>
-    <row r="130" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A130" s="1" t="s">
         <v>346</v>
       </c>
@@ -7702,10 +7702,10 @@
         <v>349</v>
       </c>
       <c r="F130" s="1" t="s">
-        <v>1535</v>
-      </c>
-    </row>
-    <row r="131" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+        <v>1534</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A131" s="1" t="s">
         <v>350</v>
       </c>
@@ -7720,10 +7720,10 @@
         <v>352</v>
       </c>
       <c r="F131" s="1" t="s">
-        <v>1536</v>
-      </c>
-    </row>
-    <row r="132" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+        <v>1535</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A132" s="1" t="s">
         <v>353</v>
       </c>
@@ -7741,7 +7741,7 @@
         <v>1398</v>
       </c>
     </row>
-    <row r="133" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A133" s="1" t="s">
         <v>357</v>
       </c>
@@ -7759,7 +7759,7 @@
         <v>1398</v>
       </c>
     </row>
-    <row r="134" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A134" s="1" t="s">
         <v>359</v>
       </c>
@@ -7777,7 +7777,7 @@
         <v>1398</v>
       </c>
     </row>
-    <row r="135" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A135" s="1" t="s">
         <v>361</v>
       </c>
@@ -7795,7 +7795,7 @@
         <v>1398</v>
       </c>
     </row>
-    <row r="136" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A136" s="1" t="s">
         <v>363</v>
       </c>
@@ -7813,7 +7813,7 @@
         <v>1398</v>
       </c>
     </row>
-    <row r="137" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A137" s="1" t="s">
         <v>365</v>
       </c>
@@ -7831,7 +7831,7 @@
         <v>1398</v>
       </c>
     </row>
-    <row r="138" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A138" s="1" t="s">
         <v>367</v>
       </c>
@@ -7849,7 +7849,7 @@
         <v>1399</v>
       </c>
     </row>
-    <row r="139" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A139" s="1" t="s">
         <v>370</v>
       </c>
@@ -7867,7 +7867,7 @@
         <v>1400</v>
       </c>
     </row>
-    <row r="140" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A140" s="1" t="s">
         <v>373</v>
       </c>
@@ -7885,7 +7885,7 @@
         <v>1401</v>
       </c>
     </row>
-    <row r="141" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A141" s="1" t="s">
         <v>376</v>
       </c>
@@ -7903,7 +7903,7 @@
         <v>1402</v>
       </c>
     </row>
-    <row r="142" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A142" s="1" t="s">
         <v>379</v>
       </c>
@@ -7921,7 +7921,7 @@
         <v>1403</v>
       </c>
     </row>
-    <row r="143" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A143" s="1" t="s">
         <v>382</v>
       </c>
@@ -7939,7 +7939,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="144" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A144" s="1" t="s">
         <v>385</v>
       </c>
@@ -7957,7 +7957,7 @@
         <v>1404</v>
       </c>
     </row>
-    <row r="145" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A145" s="1" t="s">
         <v>388</v>
       </c>
@@ -7975,7 +7975,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="146" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A146" s="1" t="s">
         <v>391</v>
       </c>
@@ -7993,7 +7993,7 @@
         <v>1405</v>
       </c>
     </row>
-    <row r="147" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A147" s="1" t="s">
         <v>394</v>
       </c>
@@ -8011,7 +8011,7 @@
         <v>1290</v>
       </c>
     </row>
-    <row r="148" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A148" s="1" t="s">
         <v>397</v>
       </c>
@@ -8029,7 +8029,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="149" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A149" s="1" t="s">
         <v>399</v>
       </c>
@@ -8047,7 +8047,7 @@
         <v>1407</v>
       </c>
     </row>
-    <row r="150" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A150" s="1" t="s">
         <v>402</v>
       </c>
@@ -8065,7 +8065,7 @@
         <v>1408</v>
       </c>
     </row>
-    <row r="151" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A151" s="1" t="s">
         <v>404</v>
       </c>
@@ -8083,7 +8083,7 @@
         <v>1409</v>
       </c>
     </row>
-    <row r="152" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A152" s="1" t="s">
         <v>407</v>
       </c>
@@ -8101,7 +8101,7 @@
         <v>1410</v>
       </c>
     </row>
-    <row r="153" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A153" s="1" t="s">
         <v>409</v>
       </c>
@@ -8119,7 +8119,7 @@
         <v>1411</v>
       </c>
     </row>
-    <row r="154" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A154" s="1" t="s">
         <v>412</v>
       </c>
@@ -8137,7 +8137,7 @@
         <v>1412</v>
       </c>
     </row>
-    <row r="155" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A155" s="1" t="s">
         <v>414</v>
       </c>
@@ -8155,7 +8155,7 @@
         <v>1413</v>
       </c>
     </row>
-    <row r="156" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A156" s="1" t="s">
         <v>417</v>
       </c>
@@ -8173,7 +8173,7 @@
         <v>1414</v>
       </c>
     </row>
-    <row r="157" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A157" s="1" t="s">
         <v>420</v>
       </c>
@@ -8191,7 +8191,7 @@
         <v>1415</v>
       </c>
     </row>
-    <row r="158" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A158" s="1" t="s">
         <v>423</v>
       </c>
@@ -8209,7 +8209,7 @@
         <v>1416</v>
       </c>
     </row>
-    <row r="159" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A159" s="1" t="s">
         <v>426</v>
       </c>
@@ -8227,7 +8227,7 @@
         <v>1417</v>
       </c>
     </row>
-    <row r="160" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A160" s="1" t="s">
         <v>429</v>
       </c>
@@ -8245,7 +8245,7 @@
         <v>1418</v>
       </c>
     </row>
-    <row r="161" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A161" s="1" t="s">
         <v>432</v>
       </c>
@@ -8263,7 +8263,7 @@
         <v>1419</v>
       </c>
     </row>
-    <row r="162" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A162" s="1" t="s">
         <v>435</v>
       </c>
@@ -8281,7 +8281,7 @@
         <v>1420</v>
       </c>
     </row>
-    <row r="163" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A163" s="1" t="s">
         <v>438</v>
       </c>
@@ -8299,7 +8299,7 @@
         <v>1304</v>
       </c>
     </row>
-    <row r="164" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A164" s="1" t="s">
         <v>441</v>
       </c>
@@ -8317,7 +8317,7 @@
         <v>1421</v>
       </c>
     </row>
-    <row r="165" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A165" s="1" t="s">
         <v>444</v>
       </c>
@@ -8335,7 +8335,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="166" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A166" s="1" t="s">
         <v>447</v>
       </c>
@@ -8353,7 +8353,7 @@
         <v>1291</v>
       </c>
     </row>
-    <row r="167" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A167" s="1" t="s">
         <v>450</v>
       </c>
@@ -8371,7 +8371,7 @@
         <v>1423</v>
       </c>
     </row>
-    <row r="168" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A168" s="1" t="s">
         <v>453</v>
       </c>
@@ -8389,7 +8389,7 @@
         <v>1424</v>
       </c>
     </row>
-    <row r="169" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A169" s="1" t="s">
         <v>456</v>
       </c>
@@ -8407,7 +8407,7 @@
         <v>1401</v>
       </c>
     </row>
-    <row r="170" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A170" s="1" t="s">
         <v>458</v>
       </c>
@@ -8425,7 +8425,7 @@
         <v>1292</v>
       </c>
     </row>
-    <row r="171" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A171" s="1" t="s">
         <v>461</v>
       </c>
@@ -8443,7 +8443,7 @@
         <v>1425</v>
       </c>
     </row>
-    <row r="172" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A172" s="1" t="s">
         <v>464</v>
       </c>
@@ -8461,7 +8461,7 @@
         <v>1293</v>
       </c>
     </row>
-    <row r="173" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A173" s="1" t="s">
         <v>467</v>
       </c>
@@ -8479,7 +8479,7 @@
         <v>1404</v>
       </c>
     </row>
-    <row r="174" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A174" s="1" t="s">
         <v>469</v>
       </c>
@@ -8497,7 +8497,7 @@
         <v>1426</v>
       </c>
     </row>
-    <row r="175" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A175" s="1" t="s">
         <v>472</v>
       </c>
@@ -8515,7 +8515,7 @@
         <v>1427</v>
       </c>
     </row>
-    <row r="176" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A176" s="1" t="s">
         <v>475</v>
       </c>
@@ -8533,7 +8533,7 @@
         <v>1294</v>
       </c>
     </row>
-    <row r="177" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A177" s="1" t="s">
         <v>478</v>
       </c>
@@ -8551,7 +8551,7 @@
         <v>1428</v>
       </c>
     </row>
-    <row r="178" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A178" s="1" t="s">
         <v>481</v>
       </c>
@@ -8569,7 +8569,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="179" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A179" s="1" t="s">
         <v>484</v>
       </c>
@@ -8587,7 +8587,7 @@
         <v>1430</v>
       </c>
     </row>
-    <row r="180" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A180" s="1" t="s">
         <v>487</v>
       </c>
@@ -8605,7 +8605,7 @@
         <v>1431</v>
       </c>
     </row>
-    <row r="181" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A181" s="1" t="s">
         <v>490</v>
       </c>
@@ -8623,7 +8623,7 @@
         <v>1420</v>
       </c>
     </row>
-    <row r="182" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A182" s="1" t="s">
         <v>492</v>
       </c>
@@ -8641,7 +8641,7 @@
         <v>1304</v>
       </c>
     </row>
-    <row r="183" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A183" s="1" t="s">
         <v>494</v>
       </c>
@@ -8659,7 +8659,7 @@
         <v>1295</v>
       </c>
     </row>
-    <row r="184" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A184" s="1" t="s">
         <v>497</v>
       </c>
@@ -8677,7 +8677,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="185" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A185" s="1" t="s">
         <v>499</v>
       </c>
@@ -8695,7 +8695,7 @@
         <v>1432</v>
       </c>
     </row>
-    <row r="186" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A186" s="1" t="s">
         <v>502</v>
       </c>
@@ -8713,7 +8713,7 @@
         <v>1433</v>
       </c>
     </row>
-    <row r="187" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A187" s="1" t="s">
         <v>505</v>
       </c>
@@ -8731,7 +8731,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="188" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A188" s="1" t="s">
         <v>507</v>
       </c>
@@ -8749,7 +8749,7 @@
         <v>1434</v>
       </c>
     </row>
-    <row r="189" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A189" s="1" t="s">
         <v>510</v>
       </c>
@@ -8767,7 +8767,7 @@
         <v>1431</v>
       </c>
     </row>
-    <row r="190" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A190" s="1" t="s">
         <v>512</v>
       </c>
@@ -8785,7 +8785,7 @@
         <v>1420</v>
       </c>
     </row>
-    <row r="191" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A191" s="1" t="s">
         <v>514</v>
       </c>
@@ -8803,7 +8803,7 @@
         <v>1304</v>
       </c>
     </row>
-    <row r="192" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A192" s="1" t="s">
         <v>516</v>
       </c>
@@ -8821,7 +8821,7 @@
         <v>1295</v>
       </c>
     </row>
-    <row r="193" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A193" s="1" t="s">
         <v>519</v>
       </c>
@@ -8839,7 +8839,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="194" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A194" s="1" t="s">
         <v>521</v>
       </c>
@@ -8857,7 +8857,7 @@
         <v>1432</v>
       </c>
     </row>
-    <row r="195" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A195" s="1" t="s">
         <v>523</v>
       </c>
@@ -8875,7 +8875,7 @@
         <v>1433</v>
       </c>
     </row>
-    <row r="196" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A196" s="1" t="s">
         <v>525</v>
       </c>
@@ -8893,7 +8893,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="197" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A197" s="1" t="s">
         <v>527</v>
       </c>
@@ -8911,7 +8911,7 @@
         <v>1435</v>
       </c>
     </row>
-    <row r="198" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A198" s="1" t="s">
         <v>530</v>
       </c>
@@ -8929,7 +8929,7 @@
         <v>1431</v>
       </c>
     </row>
-    <row r="199" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A199" s="1" t="s">
         <v>532</v>
       </c>
@@ -8947,7 +8947,7 @@
         <v>1420</v>
       </c>
     </row>
-    <row r="200" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A200" s="1" t="s">
         <v>534</v>
       </c>
@@ -8965,7 +8965,7 @@
         <v>1304</v>
       </c>
     </row>
-    <row r="201" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A201" s="1" t="s">
         <v>536</v>
       </c>
@@ -8983,7 +8983,7 @@
         <v>1296</v>
       </c>
     </row>
-    <row r="202" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A202" s="1" t="s">
         <v>539</v>
       </c>
@@ -9001,7 +9001,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="203" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A203" s="1" t="s">
         <v>541</v>
       </c>
@@ -9019,7 +9019,7 @@
         <v>1432</v>
       </c>
     </row>
-    <row r="204" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A204" s="1" t="s">
         <v>543</v>
       </c>
@@ -9037,7 +9037,7 @@
         <v>1343</v>
       </c>
     </row>
-    <row r="205" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A205" s="1" t="s">
         <v>546</v>
       </c>
@@ -9055,7 +9055,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="206" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A206" s="1" t="s">
         <v>548</v>
       </c>
@@ -9073,7 +9073,7 @@
         <v>1297</v>
       </c>
     </row>
-    <row r="207" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A207" s="1" t="s">
         <v>551</v>
       </c>
@@ -9091,7 +9091,7 @@
         <v>1436</v>
       </c>
     </row>
-    <row r="208" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A208" s="1" t="s">
         <v>554</v>
       </c>
@@ -9109,7 +9109,7 @@
         <v>1420</v>
       </c>
     </row>
-    <row r="209" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A209" s="1" t="s">
         <v>556</v>
       </c>
@@ -9127,7 +9127,7 @@
         <v>1304</v>
       </c>
     </row>
-    <row r="210" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A210" s="1" t="s">
         <v>558</v>
       </c>
@@ -9145,7 +9145,7 @@
         <v>1298</v>
       </c>
     </row>
-    <row r="211" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A211" s="1" t="s">
         <v>561</v>
       </c>
@@ -9163,7 +9163,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="212" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A212" s="1" t="s">
         <v>563</v>
       </c>
@@ -9181,7 +9181,7 @@
         <v>1299</v>
       </c>
     </row>
-    <row r="213" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A213" s="1" t="s">
         <v>566</v>
       </c>
@@ -9199,7 +9199,7 @@
         <v>1437</v>
       </c>
     </row>
-    <row r="214" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A214" s="1" t="s">
         <v>569</v>
       </c>
@@ -9217,7 +9217,7 @@
         <v>1438</v>
       </c>
     </row>
-    <row r="215" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A215" s="1" t="s">
         <v>572</v>
       </c>
@@ -9235,7 +9235,7 @@
         <v>1300</v>
       </c>
     </row>
-    <row r="216" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A216" s="1" t="s">
         <v>575</v>
       </c>
@@ -9253,7 +9253,7 @@
         <v>1431</v>
       </c>
     </row>
-    <row r="217" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A217" s="1" t="s">
         <v>577</v>
       </c>
@@ -9271,7 +9271,7 @@
         <v>1420</v>
       </c>
     </row>
-    <row r="218" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A218" s="1" t="s">
         <v>579</v>
       </c>
@@ -9289,7 +9289,7 @@
         <v>1304</v>
       </c>
     </row>
-    <row r="219" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A219" s="1" t="s">
         <v>581</v>
       </c>
@@ -9307,7 +9307,7 @@
         <v>1301</v>
       </c>
     </row>
-    <row r="220" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A220" s="1" t="s">
         <v>584</v>
       </c>
@@ -9325,7 +9325,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="221" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A221" s="1" t="s">
         <v>586</v>
       </c>
@@ -9343,7 +9343,7 @@
         <v>1299</v>
       </c>
     </row>
-    <row r="222" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A222" s="1" t="s">
         <v>588</v>
       </c>
@@ -9361,7 +9361,7 @@
         <v>1423</v>
       </c>
     </row>
-    <row r="223" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A223" s="1" t="s">
         <v>590</v>
       </c>
@@ -9379,7 +9379,7 @@
         <v>1439</v>
       </c>
     </row>
-    <row r="224" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A224" s="1" t="s">
         <v>593</v>
       </c>
@@ -9397,7 +9397,7 @@
         <v>1401</v>
       </c>
     </row>
-    <row r="225" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A225" s="1" t="s">
         <v>595</v>
       </c>
@@ -9415,7 +9415,7 @@
         <v>1440</v>
       </c>
     </row>
-    <row r="226" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A226" s="1" t="s">
         <v>598</v>
       </c>
@@ -9433,7 +9433,7 @@
         <v>1441</v>
       </c>
     </row>
-    <row r="227" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A227" s="1" t="s">
         <v>601</v>
       </c>
@@ -9451,7 +9451,7 @@
         <v>1442</v>
       </c>
     </row>
-    <row r="228" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A228" s="1" t="s">
         <v>604</v>
       </c>
@@ -9469,7 +9469,7 @@
         <v>1443</v>
       </c>
     </row>
-    <row r="229" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A229" s="1" t="s">
         <v>607</v>
       </c>
@@ -9487,7 +9487,7 @@
         <v>1444</v>
       </c>
     </row>
-    <row r="230" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A230" s="1" t="s">
         <v>610</v>
       </c>
@@ -9505,7 +9505,7 @@
         <v>1445</v>
       </c>
     </row>
-    <row r="231" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A231" s="1" t="s">
         <v>613</v>
       </c>
@@ -9523,7 +9523,7 @@
         <v>1302</v>
       </c>
     </row>
-    <row r="232" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A232" s="1" t="s">
         <v>616</v>
       </c>
@@ -9541,7 +9541,7 @@
         <v>1446</v>
       </c>
     </row>
-    <row r="233" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A233" s="1" t="s">
         <v>619</v>
       </c>
@@ -9559,7 +9559,7 @@
         <v>1447</v>
       </c>
     </row>
-    <row r="234" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A234" s="1" t="s">
         <v>622</v>
       </c>
@@ -9577,7 +9577,7 @@
         <v>1303</v>
       </c>
     </row>
-    <row r="235" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A235" s="1" t="s">
         <v>625</v>
       </c>
@@ -9595,7 +9595,7 @@
         <v>1448</v>
       </c>
     </row>
-    <row r="236" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A236" s="1" t="s">
         <v>627</v>
       </c>
@@ -9613,7 +9613,7 @@
         <v>1449</v>
       </c>
     </row>
-    <row r="237" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A237" s="1" t="s">
         <v>630</v>
       </c>
@@ -9631,7 +9631,7 @@
         <v>1304</v>
       </c>
     </row>
-    <row r="238" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A238" s="1" t="s">
         <v>632</v>
       </c>
@@ -9649,7 +9649,7 @@
         <v>1305</v>
       </c>
     </row>
-    <row r="239" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A239" s="1" t="s">
         <v>635</v>
       </c>
@@ -9667,7 +9667,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="240" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A240" s="1" t="s">
         <v>637</v>
       </c>
@@ -9685,7 +9685,7 @@
         <v>1306</v>
       </c>
     </row>
-    <row r="241" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A241" s="1" t="s">
         <v>640</v>
       </c>
@@ -9703,7 +9703,7 @@
         <v>1307</v>
       </c>
     </row>
-    <row r="242" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A242" s="1" t="s">
         <v>643</v>
       </c>
@@ -9721,7 +9721,7 @@
         <v>1447</v>
       </c>
     </row>
-    <row r="243" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A243" s="1" t="s">
         <v>645</v>
       </c>
@@ -9739,7 +9739,7 @@
         <v>1308</v>
       </c>
     </row>
-    <row r="244" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A244" s="1" t="s">
         <v>648</v>
       </c>
@@ -9757,7 +9757,7 @@
         <v>1448</v>
       </c>
     </row>
-    <row r="245" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A245" s="1" t="s">
         <v>650</v>
       </c>
@@ -9775,7 +9775,7 @@
         <v>1449</v>
       </c>
     </row>
-    <row r="246" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A246" s="1" t="s">
         <v>652</v>
       </c>
@@ -9793,7 +9793,7 @@
         <v>1304</v>
       </c>
     </row>
-    <row r="247" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A247" s="1" t="s">
         <v>654</v>
       </c>
@@ -9811,7 +9811,7 @@
         <v>1309</v>
       </c>
     </row>
-    <row r="248" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A248" s="1" t="s">
         <v>656</v>
       </c>
@@ -9829,7 +9829,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="249" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A249" s="1" t="s">
         <v>658</v>
       </c>
@@ -9847,7 +9847,7 @@
         <v>1306</v>
       </c>
     </row>
-    <row r="250" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A250" s="1" t="s">
         <v>661</v>
       </c>
@@ -9865,7 +9865,7 @@
         <v>1437</v>
       </c>
     </row>
-    <row r="251" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A251" s="1" t="s">
         <v>664</v>
       </c>
@@ -9883,7 +9883,7 @@
         <v>1447</v>
       </c>
     </row>
-    <row r="252" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A252" s="1" t="s">
         <v>666</v>
       </c>
@@ -9901,7 +9901,7 @@
         <v>1450</v>
       </c>
     </row>
-    <row r="253" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A253" s="1" t="s">
         <v>669</v>
       </c>
@@ -9919,7 +9919,7 @@
         <v>1431</v>
       </c>
     </row>
-    <row r="254" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A254" s="1" t="s">
         <v>671</v>
       </c>
@@ -9937,7 +9937,7 @@
         <v>1451</v>
       </c>
     </row>
-    <row r="255" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A255" s="1" t="s">
         <v>673</v>
       </c>
@@ -9955,7 +9955,7 @@
         <v>1304</v>
       </c>
     </row>
-    <row r="256" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A256" s="1" t="s">
         <v>675</v>
       </c>
@@ -9973,7 +9973,7 @@
         <v>1310</v>
       </c>
     </row>
-    <row r="257" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A257" s="1" t="s">
         <v>678</v>
       </c>
@@ -9991,7 +9991,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="258" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A258" s="1" t="s">
         <v>680</v>
       </c>
@@ -10009,7 +10009,7 @@
         <v>1452</v>
       </c>
     </row>
-    <row r="259" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="259" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A259" s="1" t="s">
         <v>683</v>
       </c>
@@ -10027,7 +10027,7 @@
         <v>1453</v>
       </c>
     </row>
-    <row r="260" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="260" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A260" s="1" t="s">
         <v>686</v>
       </c>
@@ -10045,7 +10045,7 @@
         <v>1447</v>
       </c>
     </row>
-    <row r="261" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="261" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A261" s="1" t="s">
         <v>688</v>
       </c>
@@ -10063,7 +10063,7 @@
         <v>1454</v>
       </c>
     </row>
-    <row r="262" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="262" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A262" s="1" t="s">
         <v>691</v>
       </c>
@@ -10081,7 +10081,7 @@
         <v>1455</v>
       </c>
     </row>
-    <row r="263" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="263" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A263" s="1" t="s">
         <v>693</v>
       </c>
@@ -10099,7 +10099,7 @@
         <v>1456</v>
       </c>
     </row>
-    <row r="264" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="264" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A264" s="1" t="s">
         <v>695</v>
       </c>
@@ -10117,7 +10117,7 @@
         <v>1304</v>
       </c>
     </row>
-    <row r="265" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="265" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A265" s="1" t="s">
         <v>697</v>
       </c>
@@ -10135,7 +10135,7 @@
         <v>1311</v>
       </c>
     </row>
-    <row r="266" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="266" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A266" s="1" t="s">
         <v>700</v>
       </c>
@@ -10153,7 +10153,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="267" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="267" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A267" s="1" t="s">
         <v>702</v>
       </c>
@@ -10171,7 +10171,7 @@
         <v>1312</v>
       </c>
     </row>
-    <row r="268" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="268" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A268" s="1" t="s">
         <v>705</v>
       </c>
@@ -10189,7 +10189,7 @@
         <v>1457</v>
       </c>
     </row>
-    <row r="269" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="269" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A269" s="1" t="s">
         <v>708</v>
       </c>
@@ -10207,7 +10207,7 @@
         <v>1458</v>
       </c>
     </row>
-    <row r="270" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="270" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A270" s="1" t="s">
         <v>711</v>
       </c>
@@ -10225,7 +10225,7 @@
         <v>1459</v>
       </c>
     </row>
-    <row r="271" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="271" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A271" s="1" t="s">
         <v>714</v>
       </c>
@@ -10243,7 +10243,7 @@
         <v>1460</v>
       </c>
     </row>
-    <row r="272" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="272" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A272" s="1" t="s">
         <v>717</v>
       </c>
@@ -10261,7 +10261,7 @@
         <v>1461</v>
       </c>
     </row>
-    <row r="273" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="273" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A273" s="1" t="s">
         <v>720</v>
       </c>
@@ -10279,7 +10279,7 @@
         <v>1462</v>
       </c>
     </row>
-    <row r="274" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="274" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A274" s="1" t="s">
         <v>723</v>
       </c>
@@ -10297,7 +10297,7 @@
         <v>1463</v>
       </c>
     </row>
-    <row r="275" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="275" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A275" s="1" t="s">
         <v>726</v>
       </c>
@@ -10315,7 +10315,7 @@
         <v>1464</v>
       </c>
     </row>
-    <row r="276" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="276" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A276" s="1" t="s">
         <v>729</v>
       </c>
@@ -10333,7 +10333,7 @@
         <v>1465</v>
       </c>
     </row>
-    <row r="277" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="277" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A277" s="1" t="s">
         <v>731</v>
       </c>
@@ -10351,7 +10351,7 @@
         <v>1458</v>
       </c>
     </row>
-    <row r="278" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="278" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A278" s="1" t="s">
         <v>733</v>
       </c>
@@ -10369,7 +10369,7 @@
         <v>1459</v>
       </c>
     </row>
-    <row r="279" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="279" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A279" s="1" t="s">
         <v>735</v>
       </c>
@@ -10387,7 +10387,7 @@
         <v>1313</v>
       </c>
     </row>
-    <row r="280" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="280" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A280" s="1" t="s">
         <v>738</v>
       </c>
@@ -10405,7 +10405,7 @@
         <v>1314</v>
       </c>
     </row>
-    <row r="281" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="281" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A281" s="1" t="s">
         <v>740</v>
       </c>
@@ -10423,7 +10423,7 @@
         <v>1462</v>
       </c>
     </row>
-    <row r="282" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="282" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A282" s="1" t="s">
         <v>742</v>
       </c>
@@ -10441,7 +10441,7 @@
         <v>1466</v>
       </c>
     </row>
-    <row r="283" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="283" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A283" s="1" t="s">
         <v>745</v>
       </c>
@@ -10459,7 +10459,7 @@
         <v>1464</v>
       </c>
     </row>
-    <row r="284" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="284" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A284" s="1" t="s">
         <v>747</v>
       </c>
@@ -10477,7 +10477,7 @@
         <v>1467</v>
       </c>
     </row>
-    <row r="285" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="285" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A285" s="1" t="s">
         <v>750</v>
       </c>
@@ -10495,7 +10495,7 @@
         <v>1468</v>
       </c>
     </row>
-    <row r="286" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="286" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A286" s="1" t="s">
         <v>753</v>
       </c>
@@ -10513,7 +10513,7 @@
         <v>1315</v>
       </c>
     </row>
-    <row r="287" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="287" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A287" s="1" t="s">
         <v>756</v>
       </c>
@@ -10531,7 +10531,7 @@
         <v>1316</v>
       </c>
     </row>
-    <row r="288" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="288" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A288" s="1" t="s">
         <v>759</v>
       </c>
@@ -10549,7 +10549,7 @@
         <v>1469</v>
       </c>
     </row>
-    <row r="289" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="289" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A289" s="1" t="s">
         <v>762</v>
       </c>
@@ -10567,7 +10567,7 @@
         <v>1470</v>
       </c>
     </row>
-    <row r="290" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="290" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A290" s="1" t="s">
         <v>765</v>
       </c>
@@ -10585,7 +10585,7 @@
         <v>1471</v>
       </c>
     </row>
-    <row r="291" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="291" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A291" s="1" t="s">
         <v>768</v>
       </c>
@@ -10603,7 +10603,7 @@
         <v>1472</v>
       </c>
     </row>
-    <row r="292" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="292" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A292" s="1" t="s">
         <v>771</v>
       </c>
@@ -10621,7 +10621,7 @@
         <v>1473</v>
       </c>
     </row>
-    <row r="293" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="293" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A293" s="1" t="s">
         <v>774</v>
       </c>
@@ -10639,7 +10639,7 @@
         <v>1474</v>
       </c>
     </row>
-    <row r="294" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="294" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A294" s="1" t="s">
         <v>777</v>
       </c>
@@ -10657,7 +10657,7 @@
         <v>1475</v>
       </c>
     </row>
-    <row r="295" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="295" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A295" s="1" t="s">
         <v>780</v>
       </c>
@@ -10675,7 +10675,7 @@
         <v>1476</v>
       </c>
     </row>
-    <row r="296" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="296" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A296" s="1" t="s">
         <v>783</v>
       </c>
@@ -10693,7 +10693,7 @@
         <v>1475</v>
       </c>
     </row>
-    <row r="297" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="297" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A297" s="1" t="s">
         <v>785</v>
       </c>
@@ -10711,7 +10711,7 @@
         <v>1317</v>
       </c>
     </row>
-    <row r="298" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="298" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A298" s="1" t="s">
         <v>788</v>
       </c>
@@ -10729,7 +10729,7 @@
         <v>1477</v>
       </c>
     </row>
-    <row r="299" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="299" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A299" s="1" t="s">
         <v>791</v>
       </c>
@@ -10747,7 +10747,7 @@
         <v>1478</v>
       </c>
     </row>
-    <row r="300" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="300" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A300" s="1" t="s">
         <v>794</v>
       </c>
@@ -10765,7 +10765,7 @@
         <v>1318</v>
       </c>
     </row>
-    <row r="301" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="301" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A301" s="1" t="s">
         <v>797</v>
       </c>
@@ -10783,7 +10783,7 @@
         <v>1462</v>
       </c>
     </row>
-    <row r="302" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="302" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A302" s="1" t="s">
         <v>799</v>
       </c>
@@ -10801,7 +10801,7 @@
         <v>1479</v>
       </c>
     </row>
-    <row r="303" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="303" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A303" s="1" t="s">
         <v>802</v>
       </c>
@@ -10819,7 +10819,7 @@
         <v>1457</v>
       </c>
     </row>
-    <row r="304" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="304" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A304" s="1" t="s">
         <v>804</v>
       </c>
@@ -10837,7 +10837,7 @@
         <v>1458</v>
       </c>
     </row>
-    <row r="305" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="305" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A305" s="1" t="s">
         <v>806</v>
       </c>
@@ -10855,7 +10855,7 @@
         <v>1319</v>
       </c>
     </row>
-    <row r="306" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="306" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A306" s="1" t="s">
         <v>809</v>
       </c>
@@ -10873,7 +10873,7 @@
         <v>1459</v>
       </c>
     </row>
-    <row r="307" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="307" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A307" s="1" t="s">
         <v>811</v>
       </c>
@@ -10891,7 +10891,7 @@
         <v>1464</v>
       </c>
     </row>
-    <row r="308" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="308" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A308" s="1" t="s">
         <v>813</v>
       </c>
@@ -10909,7 +10909,7 @@
         <v>1467</v>
       </c>
     </row>
-    <row r="309" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="309" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A309" s="1" t="s">
         <v>816</v>
       </c>
@@ -10927,7 +10927,7 @@
         <v>1480</v>
       </c>
     </row>
-    <row r="310" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="310" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A310" s="1" t="s">
         <v>819</v>
       </c>
@@ -10945,7 +10945,7 @@
         <v>1481</v>
       </c>
     </row>
-    <row r="311" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="311" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A311" s="1" t="s">
         <v>822</v>
       </c>
@@ -10963,7 +10963,7 @@
         <v>1314</v>
       </c>
     </row>
-    <row r="312" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="312" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A312" s="1" t="s">
         <v>825</v>
       </c>
@@ -10981,7 +10981,7 @@
         <v>1462</v>
       </c>
     </row>
-    <row r="313" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="313" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A313" s="1" t="s">
         <v>828</v>
       </c>
@@ -10999,7 +10999,7 @@
         <v>1482</v>
       </c>
     </row>
-    <row r="314" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="314" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A314" s="1" t="s">
         <v>831</v>
       </c>
@@ -11017,7 +11017,7 @@
         <v>1483</v>
       </c>
     </row>
-    <row r="315" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="315" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A315" s="1" t="s">
         <v>834</v>
       </c>
@@ -11035,7 +11035,7 @@
         <v>1484</v>
       </c>
     </row>
-    <row r="316" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="316" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A316" s="1" t="s">
         <v>837</v>
       </c>
@@ -11053,7 +11053,7 @@
         <v>1485</v>
       </c>
     </row>
-    <row r="317" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="317" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A317" s="1" t="s">
         <v>840</v>
       </c>
@@ -11071,7 +11071,7 @@
         <v>1320</v>
       </c>
     </row>
-    <row r="318" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="318" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A318" s="1" t="s">
         <v>843</v>
       </c>
@@ -11089,7 +11089,7 @@
         <v>1321</v>
       </c>
     </row>
-    <row r="319" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="319" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A319" s="1" t="s">
         <v>846</v>
       </c>
@@ -11107,7 +11107,7 @@
         <v>1322</v>
       </c>
     </row>
-    <row r="320" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="320" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A320" s="1" t="s">
         <v>849</v>
       </c>
@@ -11125,7 +11125,7 @@
         <v>1486</v>
       </c>
     </row>
-    <row r="321" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="321" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A321" s="1" t="s">
         <v>852</v>
       </c>
@@ -11143,7 +11143,7 @@
         <v>1323</v>
       </c>
     </row>
-    <row r="322" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="322" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A322" s="1" t="s">
         <v>855</v>
       </c>
@@ -11158,10 +11158,10 @@
         <v>857</v>
       </c>
       <c r="F322" s="1" t="s">
-        <v>1616</v>
-      </c>
-    </row>
-    <row r="323" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+        <v>1615</v>
+      </c>
+    </row>
+    <row r="323" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A323" s="1" t="s">
         <v>858</v>
       </c>
@@ -11179,7 +11179,7 @@
         <v>1487</v>
       </c>
     </row>
-    <row r="324" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="324" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A324" s="1" t="s">
         <v>861</v>
       </c>
@@ -11197,7 +11197,7 @@
         <v>1488</v>
       </c>
     </row>
-    <row r="325" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="325" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A325" s="1" t="s">
         <v>864</v>
       </c>
@@ -11215,7 +11215,7 @@
         <v>1324</v>
       </c>
     </row>
-    <row r="326" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="326" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A326" s="1" t="s">
         <v>867</v>
       </c>
@@ -11233,7 +11233,7 @@
         <v>1489</v>
       </c>
     </row>
-    <row r="327" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="327" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A327" s="1" t="s">
         <v>870</v>
       </c>
@@ -11251,7 +11251,7 @@
         <v>1490</v>
       </c>
     </row>
-    <row r="328" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="328" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A328" s="1" t="s">
         <v>873</v>
       </c>
@@ -11269,7 +11269,7 @@
         <v>1491</v>
       </c>
     </row>
-    <row r="329" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="329" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A329" s="1" t="s">
         <v>876</v>
       </c>
@@ -11287,7 +11287,7 @@
         <v>1492</v>
       </c>
     </row>
-    <row r="330" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="330" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A330" s="1" t="s">
         <v>879</v>
       </c>
@@ -11305,7 +11305,7 @@
         <v>1493</v>
       </c>
     </row>
-    <row r="331" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="331" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A331" s="1" t="s">
         <v>882</v>
       </c>
@@ -11323,7 +11323,7 @@
         <v>1455</v>
       </c>
     </row>
-    <row r="332" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="332" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A332" s="1" t="s">
         <v>885</v>
       </c>
@@ -11341,7 +11341,7 @@
         <v>1494</v>
       </c>
     </row>
-    <row r="333" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="333" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A333" s="1" t="s">
         <v>888</v>
       </c>
@@ -11359,7 +11359,7 @@
         <v>1304</v>
       </c>
     </row>
-    <row r="334" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="334" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A334" s="1" t="s">
         <v>890</v>
       </c>
@@ -11377,7 +11377,7 @@
         <v>1495</v>
       </c>
     </row>
-    <row r="335" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="335" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A335" s="1" t="s">
         <v>893</v>
       </c>
@@ -11395,7 +11395,7 @@
         <v>1496</v>
       </c>
     </row>
-    <row r="336" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="336" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A336" s="1" t="s">
         <v>896</v>
       </c>
@@ -11413,7 +11413,7 @@
         <v>1497</v>
       </c>
     </row>
-    <row r="337" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="337" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A337" s="1" t="s">
         <v>899</v>
       </c>
@@ -11431,7 +11431,7 @@
         <v>1498</v>
       </c>
     </row>
-    <row r="338" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="338" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A338" s="1" t="s">
         <v>902</v>
       </c>
@@ -11449,7 +11449,7 @@
         <v>1325</v>
       </c>
     </row>
-    <row r="339" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="339" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A339" s="1" t="s">
         <v>905</v>
       </c>
@@ -11467,7 +11467,7 @@
         <v>1499</v>
       </c>
     </row>
-    <row r="340" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="340" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A340" s="1" t="s">
         <v>908</v>
       </c>
@@ -11485,7 +11485,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="341" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="341" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A341" s="1" t="s">
         <v>911</v>
       </c>
@@ -11503,7 +11503,7 @@
         <v>1501</v>
       </c>
     </row>
-    <row r="342" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="342" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A342" s="1" t="s">
         <v>914</v>
       </c>
@@ -11521,7 +11521,7 @@
         <v>1502</v>
       </c>
     </row>
-    <row r="343" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="343" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A343" s="1" t="s">
         <v>917</v>
       </c>
@@ -11539,7 +11539,7 @@
         <v>1326</v>
       </c>
     </row>
-    <row r="344" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="344" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A344" s="1" t="s">
         <v>920</v>
       </c>
@@ -11557,7 +11557,7 @@
         <v>1327</v>
       </c>
     </row>
-    <row r="345" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="345" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A345" s="1" t="s">
         <v>923</v>
       </c>
@@ -11575,7 +11575,7 @@
         <v>1503</v>
       </c>
     </row>
-    <row r="346" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="346" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A346" s="1" t="s">
         <v>926</v>
       </c>
@@ -11593,7 +11593,7 @@
         <v>1504</v>
       </c>
     </row>
-    <row r="347" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="347" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A347" s="1" t="s">
         <v>929</v>
       </c>
@@ -11611,7 +11611,7 @@
         <v>1501</v>
       </c>
     </row>
-    <row r="348" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="348" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A348" s="1" t="s">
         <v>931</v>
       </c>
@@ -11629,7 +11629,7 @@
         <v>1502</v>
       </c>
     </row>
-    <row r="349" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="349" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A349" s="1" t="s">
         <v>933</v>
       </c>
@@ -11647,7 +11647,7 @@
         <v>1505</v>
       </c>
     </row>
-    <row r="350" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="350" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A350" s="1" t="s">
         <v>936</v>
       </c>
@@ -11665,7 +11665,7 @@
         <v>1506</v>
       </c>
     </row>
-    <row r="351" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="351" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A351" s="1" t="s">
         <v>939</v>
       </c>
@@ -11683,7 +11683,7 @@
         <v>1507</v>
       </c>
     </row>
-    <row r="352" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="352" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A352" s="1" t="s">
         <v>942</v>
       </c>
@@ -11701,7 +11701,7 @@
         <v>1508</v>
       </c>
     </row>
-    <row r="353" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="353" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A353" s="1" t="s">
         <v>945</v>
       </c>
@@ -11719,7 +11719,7 @@
         <v>1501</v>
       </c>
     </row>
-    <row r="354" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="354" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A354" s="1" t="s">
         <v>947</v>
       </c>
@@ -11737,7 +11737,7 @@
         <v>1502</v>
       </c>
     </row>
-    <row r="355" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="355" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A355" s="1" t="s">
         <v>949</v>
       </c>
@@ -11755,7 +11755,7 @@
         <v>1509</v>
       </c>
     </row>
-    <row r="356" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="356" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A356" s="1" t="s">
         <v>952</v>
       </c>
@@ -11773,7 +11773,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="357" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="357" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A357" s="1" t="s">
         <v>955</v>
       </c>
@@ -11788,10 +11788,10 @@
         <v>957</v>
       </c>
       <c r="F357" s="1" t="s">
-        <v>1511</v>
-      </c>
-    </row>
-    <row r="358" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+        <v>1632</v>
+      </c>
+    </row>
+    <row r="358" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A358" s="1" t="s">
         <v>958</v>
       </c>
@@ -11806,10 +11806,10 @@
         <v>960</v>
       </c>
       <c r="F358" s="1" t="s">
-        <v>1512</v>
-      </c>
-    </row>
-    <row r="359" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+        <v>1511</v>
+      </c>
+    </row>
+    <row r="359" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A359" s="1" t="s">
         <v>961</v>
       </c>
@@ -11827,7 +11827,7 @@
         <v>1501</v>
       </c>
     </row>
-    <row r="360" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="360" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A360" s="1" t="s">
         <v>963</v>
       </c>
@@ -11842,10 +11842,10 @@
         <v>916</v>
       </c>
       <c r="F360" s="1" t="s">
-        <v>1513</v>
-      </c>
-    </row>
-    <row r="361" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+        <v>1512</v>
+      </c>
+    </row>
+    <row r="361" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A361" s="1" t="s">
         <v>965</v>
       </c>
@@ -11860,10 +11860,10 @@
         <v>967</v>
       </c>
       <c r="F361" s="1" t="s">
-        <v>1514</v>
-      </c>
-    </row>
-    <row r="362" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+        <v>1513</v>
+      </c>
+    </row>
+    <row r="362" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A362" s="1" t="s">
         <v>968</v>
       </c>
@@ -11878,10 +11878,10 @@
         <v>970</v>
       </c>
       <c r="F362" s="1" t="s">
-        <v>1515</v>
-      </c>
-    </row>
-    <row r="363" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+        <v>1514</v>
+      </c>
+    </row>
+    <row r="363" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A363" s="1" t="s">
         <v>971</v>
       </c>
@@ -11896,10 +11896,10 @@
         <v>973</v>
       </c>
       <c r="F363" s="1" t="s">
-        <v>1516</v>
-      </c>
-    </row>
-    <row r="364" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+        <v>1515</v>
+      </c>
+    </row>
+    <row r="364" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A364" s="1" t="s">
         <v>974</v>
       </c>
@@ -11914,10 +11914,10 @@
         <v>976</v>
       </c>
       <c r="F364" s="1" t="s">
-        <v>1517</v>
-      </c>
-    </row>
-    <row r="365" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+        <v>1516</v>
+      </c>
+    </row>
+    <row r="365" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A365" s="1" t="s">
         <v>977</v>
       </c>
@@ -11935,7 +11935,7 @@
         <v>1501</v>
       </c>
     </row>
-    <row r="366" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="366" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A366" s="1" t="s">
         <v>979</v>
       </c>
@@ -11950,10 +11950,10 @@
         <v>916</v>
       </c>
       <c r="F366" s="1" t="s">
-        <v>1518</v>
-      </c>
-    </row>
-    <row r="367" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+        <v>1517</v>
+      </c>
+    </row>
+    <row r="367" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A367" s="1" t="s">
         <v>981</v>
       </c>
@@ -11968,10 +11968,10 @@
         <v>983</v>
       </c>
       <c r="F367" s="1" t="s">
-        <v>1519</v>
-      </c>
-    </row>
-    <row r="368" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+        <v>1518</v>
+      </c>
+    </row>
+    <row r="368" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A368" s="1" t="s">
         <v>984</v>
       </c>
@@ -11989,7 +11989,7 @@
         <v>1328</v>
       </c>
     </row>
-    <row r="369" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="369" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A369" s="1" t="s">
         <v>987</v>
       </c>
@@ -12004,10 +12004,10 @@
         <v>989</v>
       </c>
       <c r="F369" s="1" t="s">
-        <v>1520</v>
-      </c>
-    </row>
-    <row r="370" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+        <v>1519</v>
+      </c>
+    </row>
+    <row r="370" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A370" s="1" t="s">
         <v>990</v>
       </c>
@@ -12022,10 +12022,10 @@
         <v>992</v>
       </c>
       <c r="F370" s="1" t="s">
-        <v>1521</v>
-      </c>
-    </row>
-    <row r="371" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+        <v>1520</v>
+      </c>
+    </row>
+    <row r="371" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A371" s="1" t="s">
         <v>993</v>
       </c>
@@ -12043,7 +12043,7 @@
         <v>1464</v>
       </c>
     </row>
-    <row r="372" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="372" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A372" s="1" t="s">
         <v>995</v>
       </c>
@@ -12058,10 +12058,10 @@
         <v>997</v>
       </c>
       <c r="F372" s="1" t="s">
-        <v>1522</v>
-      </c>
-    </row>
-    <row r="373" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+        <v>1521</v>
+      </c>
+    </row>
+    <row r="373" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A373" s="1" t="s">
         <v>998</v>
       </c>
@@ -12076,10 +12076,10 @@
         <v>1000</v>
       </c>
       <c r="F373" s="1" t="s">
-        <v>1523</v>
-      </c>
-    </row>
-    <row r="374" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+        <v>1522</v>
+      </c>
+    </row>
+    <row r="374" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A374" s="1" t="s">
         <v>1001</v>
       </c>
@@ -12094,10 +12094,10 @@
         <v>1003</v>
       </c>
       <c r="F374" s="1" t="s">
-        <v>1524</v>
-      </c>
-    </row>
-    <row r="375" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+        <v>1523</v>
+      </c>
+    </row>
+    <row r="375" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A375" s="1" t="s">
         <v>1004</v>
       </c>
@@ -12112,10 +12112,10 @@
         <v>1006</v>
       </c>
       <c r="F375" s="1" t="s">
-        <v>1525</v>
-      </c>
-    </row>
-    <row r="376" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+        <v>1524</v>
+      </c>
+    </row>
+    <row r="376" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A376" s="1" t="s">
         <v>1007</v>
       </c>
@@ -12130,10 +12130,10 @@
         <v>1009</v>
       </c>
       <c r="F376" s="1" t="s">
-        <v>1526</v>
-      </c>
-    </row>
-    <row r="377" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+        <v>1525</v>
+      </c>
+    </row>
+    <row r="377" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A377" s="1" t="s">
         <v>1010</v>
       </c>
@@ -12148,10 +12148,10 @@
         <v>1012</v>
       </c>
       <c r="F377" s="1" t="s">
-        <v>1530</v>
-      </c>
-    </row>
-    <row r="378" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+        <v>1529</v>
+      </c>
+    </row>
+    <row r="378" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A378" s="1" t="s">
         <v>1013</v>
       </c>
@@ -12166,10 +12166,10 @@
         <v>1015</v>
       </c>
       <c r="F378" s="1" t="s">
-        <v>1527</v>
-      </c>
-    </row>
-    <row r="379" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+        <v>1526</v>
+      </c>
+    </row>
+    <row r="379" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A379" s="1" t="s">
         <v>1016</v>
       </c>
@@ -12184,10 +12184,10 @@
         <v>1018</v>
       </c>
       <c r="F379" s="1" t="s">
-        <v>1531</v>
-      </c>
-    </row>
-    <row r="380" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+        <v>1530</v>
+      </c>
+    </row>
+    <row r="380" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A380" s="1" t="s">
         <v>1019</v>
       </c>
@@ -12202,10 +12202,10 @@
         <v>1021</v>
       </c>
       <c r="F380" s="1" t="s">
-        <v>1532</v>
-      </c>
-    </row>
-    <row r="381" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+        <v>1531</v>
+      </c>
+    </row>
+    <row r="381" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A381" s="1" t="s">
         <v>1022</v>
       </c>
@@ -12220,10 +12220,10 @@
         <v>1024</v>
       </c>
       <c r="F381" s="1" t="s">
-        <v>1533</v>
-      </c>
-    </row>
-    <row r="382" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+        <v>1532</v>
+      </c>
+    </row>
+    <row r="382" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A382" s="1" t="s">
         <v>1025</v>
       </c>
@@ -12238,10 +12238,10 @@
         <v>1027</v>
       </c>
       <c r="F382" s="1" t="s">
-        <v>1534</v>
-      </c>
-    </row>
-    <row r="383" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+        <v>1533</v>
+      </c>
+    </row>
+    <row r="383" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A383" s="1" t="s">
         <v>1028</v>
       </c>
@@ -12256,10 +12256,10 @@
         <v>1031</v>
       </c>
       <c r="F383" s="1" t="s">
-        <v>1537</v>
-      </c>
-    </row>
-    <row r="384" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+        <v>1536</v>
+      </c>
+    </row>
+    <row r="384" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A384" s="1" t="s">
         <v>1032</v>
       </c>
@@ -12274,10 +12274,10 @@
         <v>1034</v>
       </c>
       <c r="F384" s="1" t="s">
-        <v>1592</v>
-      </c>
-    </row>
-    <row r="385" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+        <v>1591</v>
+      </c>
+    </row>
+    <row r="385" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A385" s="1" t="s">
         <v>1035</v>
       </c>
@@ -12292,10 +12292,10 @@
         <v>1037</v>
       </c>
       <c r="F385" s="1" t="s">
-        <v>1593</v>
-      </c>
-    </row>
-    <row r="386" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+        <v>1592</v>
+      </c>
+    </row>
+    <row r="386" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A386" s="1" t="s">
         <v>1038</v>
       </c>
@@ -12310,10 +12310,10 @@
         <v>1040</v>
       </c>
       <c r="F386" s="1" t="s">
-        <v>1538</v>
-      </c>
-    </row>
-    <row r="387" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+        <v>1537</v>
+      </c>
+    </row>
+    <row r="387" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A387" s="1" t="s">
         <v>1041</v>
       </c>
@@ -12328,10 +12328,10 @@
         <v>1043</v>
       </c>
       <c r="F387" s="1" t="s">
-        <v>1594</v>
-      </c>
-    </row>
-    <row r="388" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+        <v>1593</v>
+      </c>
+    </row>
+    <row r="388" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A388" s="1" t="s">
         <v>1044</v>
       </c>
@@ -12346,10 +12346,10 @@
         <v>1046</v>
       </c>
       <c r="F388" s="1" t="s">
-        <v>1539</v>
-      </c>
-    </row>
-    <row r="389" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+        <v>1538</v>
+      </c>
+    </row>
+    <row r="389" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A389" s="1" t="s">
         <v>1047</v>
       </c>
@@ -12364,10 +12364,10 @@
         <v>1049</v>
       </c>
       <c r="F389" s="1" t="s">
-        <v>1540</v>
-      </c>
-    </row>
-    <row r="390" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+        <v>1539</v>
+      </c>
+    </row>
+    <row r="390" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A390" s="1" t="s">
         <v>1050</v>
       </c>
@@ -12382,10 +12382,10 @@
         <v>1052</v>
       </c>
       <c r="F390" s="1" t="s">
-        <v>1569</v>
-      </c>
-    </row>
-    <row r="391" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+        <v>1568</v>
+      </c>
+    </row>
+    <row r="391" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A391" s="1" t="s">
         <v>1053</v>
       </c>
@@ -12400,10 +12400,10 @@
         <v>1055</v>
       </c>
       <c r="F391" s="1" t="s">
-        <v>1541</v>
-      </c>
-    </row>
-    <row r="392" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+        <v>1540</v>
+      </c>
+    </row>
+    <row r="392" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A392" s="1" t="s">
         <v>1056</v>
       </c>
@@ -12418,10 +12418,10 @@
         <v>1058</v>
       </c>
       <c r="F392" s="1" t="s">
-        <v>1542</v>
-      </c>
-    </row>
-    <row r="393" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+        <v>1541</v>
+      </c>
+    </row>
+    <row r="393" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A393" s="1" t="s">
         <v>1059</v>
       </c>
@@ -12436,10 +12436,10 @@
         <v>1061</v>
       </c>
       <c r="F393" s="1" t="s">
-        <v>1595</v>
-      </c>
-    </row>
-    <row r="394" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+        <v>1594</v>
+      </c>
+    </row>
+    <row r="394" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A394" s="1" t="s">
         <v>1062</v>
       </c>
@@ -12454,10 +12454,10 @@
         <v>1064</v>
       </c>
       <c r="F394" s="1" t="s">
-        <v>1570</v>
-      </c>
-    </row>
-    <row r="395" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+        <v>1569</v>
+      </c>
+    </row>
+    <row r="395" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A395" s="1" t="s">
         <v>1065</v>
       </c>
@@ -12472,10 +12472,10 @@
         <v>1067</v>
       </c>
       <c r="F395" s="1" t="s">
-        <v>1596</v>
-      </c>
-    </row>
-    <row r="396" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+        <v>1595</v>
+      </c>
+    </row>
+    <row r="396" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A396" s="1" t="s">
         <v>1068</v>
       </c>
@@ -12490,10 +12490,10 @@
         <v>1070</v>
       </c>
       <c r="F396" s="1" t="s">
-        <v>1597</v>
-      </c>
-    </row>
-    <row r="397" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+        <v>1596</v>
+      </c>
+    </row>
+    <row r="397" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A397" s="1" t="s">
         <v>1071</v>
       </c>
@@ -12508,10 +12508,10 @@
         <v>1073</v>
       </c>
       <c r="F397" s="1" t="s">
-        <v>1544</v>
-      </c>
-    </row>
-    <row r="398" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+        <v>1543</v>
+      </c>
+    </row>
+    <row r="398" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A398" s="1" t="s">
         <v>1074</v>
       </c>
@@ -12526,10 +12526,10 @@
         <v>1076</v>
       </c>
       <c r="F398" s="1" t="s">
-        <v>1545</v>
-      </c>
-    </row>
-    <row r="399" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+        <v>1544</v>
+      </c>
+    </row>
+    <row r="399" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A399" s="1" t="s">
         <v>1077</v>
       </c>
@@ -12544,10 +12544,10 @@
         <v>1079</v>
       </c>
       <c r="F399" s="1" t="s">
-        <v>1546</v>
-      </c>
-    </row>
-    <row r="400" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+        <v>1545</v>
+      </c>
+    </row>
+    <row r="400" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A400" s="1" t="s">
         <v>1080</v>
       </c>
@@ -12562,10 +12562,10 @@
         <v>1082</v>
       </c>
       <c r="F400" s="1" t="s">
-        <v>1547</v>
-      </c>
-    </row>
-    <row r="401" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+        <v>1546</v>
+      </c>
+    </row>
+    <row r="401" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A401" s="1" t="s">
         <v>1083</v>
       </c>
@@ -12580,10 +12580,10 @@
         <v>1085</v>
       </c>
       <c r="F401" s="1" t="s">
-        <v>1548</v>
-      </c>
-    </row>
-    <row r="402" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+        <v>1547</v>
+      </c>
+    </row>
+    <row r="402" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A402" s="1" t="s">
         <v>1086</v>
       </c>
@@ -12598,10 +12598,10 @@
         <v>1088</v>
       </c>
       <c r="F402" s="1" t="s">
-        <v>1549</v>
-      </c>
-    </row>
-    <row r="403" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+        <v>1548</v>
+      </c>
+    </row>
+    <row r="403" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A403" s="1" t="s">
         <v>1089</v>
       </c>
@@ -12616,10 +12616,10 @@
         <v>1091</v>
       </c>
       <c r="F403" s="1" t="s">
-        <v>1550</v>
-      </c>
-    </row>
-    <row r="404" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+        <v>1549</v>
+      </c>
+    </row>
+    <row r="404" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A404" s="1" t="s">
         <v>1092</v>
       </c>
@@ -12634,10 +12634,10 @@
         <v>1094</v>
       </c>
       <c r="F404" s="1" t="s">
-        <v>1551</v>
-      </c>
-    </row>
-    <row r="405" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+        <v>1550</v>
+      </c>
+    </row>
+    <row r="405" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A405" s="1" t="s">
         <v>1095</v>
       </c>
@@ -12652,10 +12652,10 @@
         <v>1097</v>
       </c>
       <c r="F405" s="1" t="s">
-        <v>1571</v>
-      </c>
-    </row>
-    <row r="406" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+        <v>1570</v>
+      </c>
+    </row>
+    <row r="406" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A406" s="1" t="s">
         <v>1098</v>
       </c>
@@ -12670,10 +12670,10 @@
         <v>1100</v>
       </c>
       <c r="F406" s="1" t="s">
-        <v>1572</v>
-      </c>
-    </row>
-    <row r="407" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+        <v>1571</v>
+      </c>
+    </row>
+    <row r="407" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A407" s="1" t="s">
         <v>1101</v>
       </c>
@@ -12688,10 +12688,10 @@
         <v>1103</v>
       </c>
       <c r="F407" s="1" t="s">
-        <v>1573</v>
-      </c>
-    </row>
-    <row r="408" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+        <v>1572</v>
+      </c>
+    </row>
+    <row r="408" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A408" s="1" t="s">
         <v>1104</v>
       </c>
@@ -12706,10 +12706,10 @@
         <v>1106</v>
       </c>
       <c r="F408" s="1" t="s">
-        <v>1576</v>
-      </c>
-    </row>
-    <row r="409" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+        <v>1575</v>
+      </c>
+    </row>
+    <row r="409" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A409" s="1" t="s">
         <v>1107</v>
       </c>
@@ -12724,10 +12724,10 @@
         <v>1109</v>
       </c>
       <c r="F409" s="1" t="s">
-        <v>1598</v>
-      </c>
-    </row>
-    <row r="410" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+        <v>1597</v>
+      </c>
+    </row>
+    <row r="410" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A410" s="1" t="s">
         <v>1110</v>
       </c>
@@ -12742,10 +12742,10 @@
         <v>1112</v>
       </c>
       <c r="F410" s="1" t="s">
-        <v>1574</v>
-      </c>
-    </row>
-    <row r="411" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+        <v>1573</v>
+      </c>
+    </row>
+    <row r="411" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A411" s="1" t="s">
         <v>1113</v>
       </c>
@@ -12760,10 +12760,10 @@
         <v>1115</v>
       </c>
       <c r="F411" s="1" t="s">
-        <v>1599</v>
-      </c>
-    </row>
-    <row r="412" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+        <v>1598</v>
+      </c>
+    </row>
+    <row r="412" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A412" s="1" t="s">
         <v>1116</v>
       </c>
@@ -12778,10 +12778,10 @@
         <v>1118</v>
       </c>
       <c r="F412" s="1" t="s">
-        <v>1600</v>
-      </c>
-    </row>
-    <row r="413" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+        <v>1599</v>
+      </c>
+    </row>
+    <row r="413" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A413" s="1" t="s">
         <v>1119</v>
       </c>
@@ -12796,10 +12796,10 @@
         <v>1121</v>
       </c>
       <c r="F413" s="1" t="s">
-        <v>1601</v>
-      </c>
-    </row>
-    <row r="414" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+        <v>1600</v>
+      </c>
+    </row>
+    <row r="414" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A414" s="1" t="s">
         <v>1122</v>
       </c>
@@ -12814,10 +12814,10 @@
         <v>1124</v>
       </c>
       <c r="F414" s="1" t="s">
-        <v>1552</v>
-      </c>
-    </row>
-    <row r="415" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+        <v>1551</v>
+      </c>
+    </row>
+    <row r="415" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A415" s="1" t="s">
         <v>1125</v>
       </c>
@@ -12832,10 +12832,10 @@
         <v>1127</v>
       </c>
       <c r="F415" s="1" t="s">
-        <v>1553</v>
-      </c>
-    </row>
-    <row r="416" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+        <v>1552</v>
+      </c>
+    </row>
+    <row r="416" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A416" s="1" t="s">
         <v>1128</v>
       </c>
@@ -12850,10 +12850,10 @@
         <v>1130</v>
       </c>
       <c r="F416" s="1" t="s">
-        <v>1554</v>
-      </c>
-    </row>
-    <row r="417" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+        <v>1553</v>
+      </c>
+    </row>
+    <row r="417" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A417" s="1" t="s">
         <v>1131</v>
       </c>
@@ -12868,10 +12868,10 @@
         <v>1133</v>
       </c>
       <c r="F417" s="1" t="s">
-        <v>1603</v>
-      </c>
-    </row>
-    <row r="418" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+        <v>1602</v>
+      </c>
+    </row>
+    <row r="418" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A418" s="1" t="s">
         <v>1134</v>
       </c>
@@ -12886,10 +12886,10 @@
         <v>1136</v>
       </c>
       <c r="F418" s="1" t="s">
-        <v>1556</v>
-      </c>
-    </row>
-    <row r="419" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+        <v>1555</v>
+      </c>
+    </row>
+    <row r="419" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A419" s="1" t="s">
         <v>1137</v>
       </c>
@@ -12904,10 +12904,10 @@
         <v>1139</v>
       </c>
       <c r="F419" s="1" t="s">
-        <v>1577</v>
-      </c>
-    </row>
-    <row r="420" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+        <v>1576</v>
+      </c>
+    </row>
+    <row r="420" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A420" s="1" t="s">
         <v>1140</v>
       </c>
@@ -12922,10 +12922,10 @@
         <v>1142</v>
       </c>
       <c r="F420" s="1" t="s">
-        <v>1602</v>
-      </c>
-    </row>
-    <row r="421" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+        <v>1601</v>
+      </c>
+    </row>
+    <row r="421" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A421" s="1" t="s">
         <v>1143</v>
       </c>
@@ -12940,10 +12940,10 @@
         <v>1145</v>
       </c>
       <c r="F421" s="1" t="s">
-        <v>1604</v>
-      </c>
-    </row>
-    <row r="422" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+        <v>1603</v>
+      </c>
+    </row>
+    <row r="422" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A422" s="1" t="s">
         <v>1146</v>
       </c>
@@ -12958,10 +12958,10 @@
         <v>1148</v>
       </c>
       <c r="F422" s="1" t="s">
-        <v>1605</v>
-      </c>
-    </row>
-    <row r="423" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+        <v>1604</v>
+      </c>
+    </row>
+    <row r="423" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A423" s="1" t="s">
         <v>1149</v>
       </c>
@@ -12976,10 +12976,10 @@
         <v>1151</v>
       </c>
       <c r="F423" s="1" t="s">
-        <v>1590</v>
-      </c>
-    </row>
-    <row r="424" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+        <v>1589</v>
+      </c>
+    </row>
+    <row r="424" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A424" s="1" t="s">
         <v>1152</v>
       </c>
@@ -12994,10 +12994,10 @@
         <v>1154</v>
       </c>
       <c r="F424" s="1" t="s">
-        <v>1557</v>
-      </c>
-    </row>
-    <row r="425" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+        <v>1556</v>
+      </c>
+    </row>
+    <row r="425" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A425" s="1" t="s">
         <v>1155</v>
       </c>
@@ -13012,10 +13012,10 @@
         <v>1157</v>
       </c>
       <c r="F425" s="1" t="s">
-        <v>1606</v>
-      </c>
-    </row>
-    <row r="426" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+        <v>1605</v>
+      </c>
+    </row>
+    <row r="426" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A426" s="1" t="s">
         <v>1158</v>
       </c>
@@ -13030,10 +13030,10 @@
         <v>1160</v>
       </c>
       <c r="F426" s="1" t="s">
-        <v>1558</v>
-      </c>
-    </row>
-    <row r="427" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+        <v>1557</v>
+      </c>
+    </row>
+    <row r="427" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A427" s="1" t="s">
         <v>1161</v>
       </c>
@@ -13048,10 +13048,10 @@
         <v>1163</v>
       </c>
       <c r="F427" s="1" t="s">
-        <v>1559</v>
-      </c>
-    </row>
-    <row r="428" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+        <v>1558</v>
+      </c>
+    </row>
+    <row r="428" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A428" s="1" t="s">
         <v>1164</v>
       </c>
@@ -13066,10 +13066,10 @@
         <v>1166</v>
       </c>
       <c r="F428" s="1" t="s">
-        <v>1560</v>
-      </c>
-    </row>
-    <row r="429" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+        <v>1559</v>
+      </c>
+    </row>
+    <row r="429" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A429" s="1" t="s">
         <v>1167</v>
       </c>
@@ -13084,10 +13084,10 @@
         <v>1169</v>
       </c>
       <c r="F429" s="1" t="s">
-        <v>1578</v>
-      </c>
-    </row>
-    <row r="430" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+        <v>1577</v>
+      </c>
+    </row>
+    <row r="430" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A430" s="1" t="s">
         <v>1170</v>
       </c>
@@ -13102,10 +13102,10 @@
         <v>1172</v>
       </c>
       <c r="F430" s="1" t="s">
-        <v>1607</v>
-      </c>
-    </row>
-    <row r="431" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+        <v>1606</v>
+      </c>
+    </row>
+    <row r="431" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A431" s="1" t="s">
         <v>1173</v>
       </c>
@@ -13120,10 +13120,10 @@
         <v>1175</v>
       </c>
       <c r="F431" s="1" t="s">
-        <v>1579</v>
-      </c>
-    </row>
-    <row r="432" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+        <v>1578</v>
+      </c>
+    </row>
+    <row r="432" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A432" s="1" t="s">
         <v>1176</v>
       </c>
@@ -13138,10 +13138,10 @@
         <v>1178</v>
       </c>
       <c r="F432" s="1" t="s">
-        <v>1608</v>
-      </c>
-    </row>
-    <row r="433" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+        <v>1607</v>
+      </c>
+    </row>
+    <row r="433" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A433" s="1" t="s">
         <v>1179</v>
       </c>
@@ -13156,10 +13156,10 @@
         <v>1181</v>
       </c>
       <c r="F433" s="1" t="s">
-        <v>1609</v>
-      </c>
-    </row>
-    <row r="434" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+        <v>1608</v>
+      </c>
+    </row>
+    <row r="434" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A434" s="1" t="s">
         <v>1182</v>
       </c>
@@ -13174,10 +13174,10 @@
         <v>1184</v>
       </c>
       <c r="F434" s="1" t="s">
-        <v>1589</v>
-      </c>
-    </row>
-    <row r="435" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+        <v>1588</v>
+      </c>
+    </row>
+    <row r="435" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A435" s="1" t="s">
         <v>1185</v>
       </c>
@@ -13192,10 +13192,10 @@
         <v>1187</v>
       </c>
       <c r="F435" s="1" t="s">
-        <v>1610</v>
-      </c>
-    </row>
-    <row r="436" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+        <v>1609</v>
+      </c>
+    </row>
+    <row r="436" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A436" s="1" t="s">
         <v>1188</v>
       </c>
@@ -13210,10 +13210,10 @@
         <v>1190</v>
       </c>
       <c r="F436" s="1" t="s">
-        <v>1580</v>
-      </c>
-    </row>
-    <row r="437" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+        <v>1579</v>
+      </c>
+    </row>
+    <row r="437" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A437" s="1" t="s">
         <v>1191</v>
       </c>
@@ -13228,10 +13228,10 @@
         <v>1193</v>
       </c>
       <c r="F437" s="1" t="s">
-        <v>1591</v>
-      </c>
-    </row>
-    <row r="438" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+        <v>1590</v>
+      </c>
+    </row>
+    <row r="438" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A438" s="1" t="s">
         <v>1194</v>
       </c>
@@ -13246,10 +13246,10 @@
         <v>1196</v>
       </c>
       <c r="F438" s="1" t="s">
-        <v>1575</v>
-      </c>
-    </row>
-    <row r="439" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+        <v>1574</v>
+      </c>
+    </row>
+    <row r="439" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A439" s="1" t="s">
         <v>1197</v>
       </c>
@@ -13264,10 +13264,10 @@
         <v>1199</v>
       </c>
       <c r="F439" s="1" t="s">
-        <v>1582</v>
-      </c>
-    </row>
-    <row r="440" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+        <v>1581</v>
+      </c>
+    </row>
+    <row r="440" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A440" s="1" t="s">
         <v>1200</v>
       </c>
@@ -13282,10 +13282,10 @@
         <v>1202</v>
       </c>
       <c r="F440" s="1" t="s">
-        <v>1583</v>
-      </c>
-    </row>
-    <row r="441" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+        <v>1582</v>
+      </c>
+    </row>
+    <row r="441" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A441" s="1" t="s">
         <v>1203</v>
       </c>
@@ -13300,10 +13300,10 @@
         <v>1205</v>
       </c>
       <c r="F441" s="1" t="s">
-        <v>1585</v>
-      </c>
-    </row>
-    <row r="442" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+        <v>1584</v>
+      </c>
+    </row>
+    <row r="442" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A442" s="1" t="s">
         <v>1206</v>
       </c>
@@ -13318,10 +13318,10 @@
         <v>1208</v>
       </c>
       <c r="F442" s="1" t="s">
-        <v>1611</v>
-      </c>
-    </row>
-    <row r="443" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+        <v>1610</v>
+      </c>
+    </row>
+    <row r="443" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A443" s="1" t="s">
         <v>1209</v>
       </c>
@@ -13336,10 +13336,10 @@
         <v>1211</v>
       </c>
       <c r="F443" s="1" t="s">
-        <v>1561</v>
-      </c>
-    </row>
-    <row r="444" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+        <v>1560</v>
+      </c>
+    </row>
+    <row r="444" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A444" s="1" t="s">
         <v>1212</v>
       </c>
@@ -13354,10 +13354,10 @@
         <v>1214</v>
       </c>
       <c r="F444" s="1" t="s">
-        <v>1562</v>
-      </c>
-    </row>
-    <row r="445" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+        <v>1561</v>
+      </c>
+    </row>
+    <row r="445" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A445" s="1" t="s">
         <v>1215</v>
       </c>
@@ -13372,10 +13372,10 @@
         <v>1217</v>
       </c>
       <c r="F445" s="1" t="s">
-        <v>1563</v>
-      </c>
-    </row>
-    <row r="446" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+        <v>1562</v>
+      </c>
+    </row>
+    <row r="446" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A446" s="1" t="s">
         <v>1218</v>
       </c>
@@ -13390,10 +13390,10 @@
         <v>1220</v>
       </c>
       <c r="F446" s="1" t="s">
-        <v>1564</v>
-      </c>
-    </row>
-    <row r="447" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+        <v>1563</v>
+      </c>
+    </row>
+    <row r="447" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A447" s="1" t="s">
         <v>1221</v>
       </c>
@@ -13408,10 +13408,10 @@
         <v>1223</v>
       </c>
       <c r="F447" s="1" t="s">
-        <v>1584</v>
-      </c>
-    </row>
-    <row r="448" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+        <v>1583</v>
+      </c>
+    </row>
+    <row r="448" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A448" s="1" t="s">
         <v>1224</v>
       </c>
@@ -13426,10 +13426,10 @@
         <v>1226</v>
       </c>
       <c r="F448" s="1" t="s">
-        <v>1586</v>
-      </c>
-    </row>
-    <row r="449" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+        <v>1585</v>
+      </c>
+    </row>
+    <row r="449" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A449" s="1" t="s">
         <v>1227</v>
       </c>
@@ -13444,10 +13444,10 @@
         <v>1229</v>
       </c>
       <c r="F449" s="1" t="s">
-        <v>1538</v>
-      </c>
-    </row>
-    <row r="450" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+        <v>1537</v>
+      </c>
+    </row>
+    <row r="450" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A450" s="1" t="s">
         <v>1230</v>
       </c>
@@ -13462,10 +13462,10 @@
         <v>1232</v>
       </c>
       <c r="F450" s="1" t="s">
-        <v>1555</v>
-      </c>
-    </row>
-    <row r="451" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+        <v>1554</v>
+      </c>
+    </row>
+    <row r="451" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A451" s="1" t="s">
         <v>1233</v>
       </c>
@@ -13480,10 +13480,10 @@
         <v>1235</v>
       </c>
       <c r="F451" s="1" t="s">
-        <v>1612</v>
-      </c>
-    </row>
-    <row r="452" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+        <v>1611</v>
+      </c>
+    </row>
+    <row r="452" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A452" s="1" t="s">
         <v>1236</v>
       </c>
@@ -13498,10 +13498,10 @@
         <v>1238</v>
       </c>
       <c r="F452" s="1" t="s">
-        <v>1613</v>
-      </c>
-    </row>
-    <row r="453" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+        <v>1612</v>
+      </c>
+    </row>
+    <row r="453" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A453" s="1" t="s">
         <v>1239</v>
       </c>
@@ -13516,10 +13516,10 @@
         <v>1241</v>
       </c>
       <c r="F453" s="1" t="s">
-        <v>1614</v>
-      </c>
-    </row>
-    <row r="454" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+        <v>1613</v>
+      </c>
+    </row>
+    <row r="454" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A454" s="1" t="s">
         <v>1242</v>
       </c>
@@ -13534,10 +13534,10 @@
         <v>1244</v>
       </c>
       <c r="F454" s="1" t="s">
-        <v>1565</v>
-      </c>
-    </row>
-    <row r="455" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+        <v>1564</v>
+      </c>
+    </row>
+    <row r="455" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A455" s="1" t="s">
         <v>1245</v>
       </c>
@@ -13552,10 +13552,10 @@
         <v>1247</v>
       </c>
       <c r="F455" s="1" t="s">
-        <v>1566</v>
-      </c>
-    </row>
-    <row r="456" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+        <v>1565</v>
+      </c>
+    </row>
+    <row r="456" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A456" s="1" t="s">
         <v>1248</v>
       </c>
@@ -13570,10 +13570,10 @@
         <v>1250</v>
       </c>
       <c r="F456" s="1" t="s">
-        <v>1615</v>
-      </c>
-    </row>
-    <row r="457" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+        <v>1614</v>
+      </c>
+    </row>
+    <row r="457" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A457" s="1" t="s">
         <v>1251</v>
       </c>
@@ -13588,10 +13588,10 @@
         <v>1253</v>
       </c>
       <c r="F457" s="1" t="s">
-        <v>1581</v>
-      </c>
-    </row>
-    <row r="458" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+        <v>1580</v>
+      </c>
+    </row>
+    <row r="458" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A458" s="1" t="s">
         <v>1254</v>
       </c>
@@ -13606,10 +13606,10 @@
         <v>1256</v>
       </c>
       <c r="F458" s="1" t="s">
-        <v>1567</v>
-      </c>
-    </row>
-    <row r="459" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+        <v>1566</v>
+      </c>
+    </row>
+    <row r="459" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A459" s="1" t="s">
         <v>1257</v>
       </c>
@@ -13624,10 +13624,10 @@
         <v>1259</v>
       </c>
       <c r="F459" s="1" t="s">
-        <v>1543</v>
-      </c>
-    </row>
-    <row r="460" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+        <v>1542</v>
+      </c>
+    </row>
+    <row r="460" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A460" s="1" t="s">
         <v>1260</v>
       </c>
@@ -13642,10 +13642,10 @@
         <v>1262</v>
       </c>
       <c r="F460" s="1" t="s">
-        <v>1568</v>
-      </c>
-    </row>
-    <row r="461" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+        <v>1567</v>
+      </c>
+    </row>
+    <row r="461" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A461" s="1" t="s">
         <v>1263</v>
       </c>
@@ -13660,10 +13660,10 @@
         <v>1265</v>
       </c>
       <c r="F461" s="1" t="s">
-        <v>1587</v>
-      </c>
-    </row>
-    <row r="462" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+        <v>1586</v>
+      </c>
+    </row>
+    <row r="462" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A462" s="1" t="s">
         <v>1266</v>
       </c>
@@ -13678,7 +13678,7 @@
         <v>1268</v>
       </c>
       <c r="F462" s="1" t="s">
-        <v>1588</v>
+        <v>1587</v>
       </c>
     </row>
   </sheetData>

</xml_diff>